<commit_message>
Framework updated. Added Random Generator classes. Add Different format attachment capability
</commit_message>
<xml_diff>
--- a/resources/ETNATestData.xlsx
+++ b/resources/ETNATestData.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17224"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanthsridhar/Projects/UnilogProjects/autframework/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest1" sheetId="1" r:id="rId1"/>
-    <sheet name="loginTest2" sheetId="2" r:id="rId2"/>
+    <sheet name="attachmentsTest1" sheetId="3" r:id="rId2"/>
+    <sheet name="loginTest2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -72,13 +83,49 @@
   </si>
   <si>
     <t>hemanth126</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>xml</t>
+  </si>
+  <si>
+    <t>txt</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>resources/TestData/sample.json</t>
+  </si>
+  <si>
+    <t>resources/TestData/sample.xlsx</t>
+  </si>
+  <si>
+    <t>resources/TestData/sample.xml</t>
+  </si>
+  <si>
+    <t>resources/TestData/sample.txt</t>
+  </si>
+  <si>
+    <t>resources/TestData/sample.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +149,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,8 +178,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DB4E2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -127,16 +195,53 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -145,11 +250,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -244,23 +353,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -296,23 +388,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,19 +542,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -517,21 +592,88 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -559,7 +701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -573,7 +715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -587,7 +729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -604,7 +746,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3:B4" r:id="rId2"/>
+    <hyperlink ref="B3:B4" r:id="rId2" display="hemanth.bs123@unilogcorp.com2"/>
     <hyperlink ref="B5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>